<commit_message>
Apply light elegant theme with red accents (#2)
* Refactor: Update styles for a cleaner, modern look

Co-authored-by: nguyentuandanh.7 <nguyentuandanh.7@gmail.com>

* Refactor: Update project section and assignee styles

Co-authored-by: nguyentuandanh.7 <nguyentuandanh.7@gmail.com>

* Refactor: Adjust card borders and shadows for lighter appearance

Co-authored-by: nguyentuandanh.7 <nguyentuandanh.7@gmail.com>

* Refactor header styles and add RMIT logo

Co-authored-by: nguyentuandanh.7 <nguyentuandanh.7@gmail.com>

* Add files via upload

* Add files via upload

* Add last modified date to Excel file processing

Co-authored-by: nguyentuandanh.7 <nguyentuandanh.7@gmail.com>

* Add server setup and file stats endpoints

Co-authored-by: nguyentuandanh.7 <nguyentuandanh.7@gmail.com>

* Remove unused file-stats endpoints and simplify index.html

Co-authored-by: nguyentuandanh.7 <nguyentuandanh.7@gmail.com>

---------

Co-authored-by: Cursor Agent <cursoragent@cursor.com>
</commit_message>
<xml_diff>
--- a/data/wip.xlsx
+++ b/data/wip.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\RMIT_WORKS\TEAM\WIP\HTML email\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A0AE85E-807A-4FDA-83E3-432E259CC1FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA2EA3D9-1FCE-4E93-A459-3DE6185C6A79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="733" yWindow="-118" windowWidth="32898" windowHeight="21181" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="66">
   <si>
     <t>Week 45 (4-11 Nov 2025)</t>
   </si>
@@ -60,9 +60,6 @@
     <t>Details</t>
   </si>
   <si>
-    <t>COP 2025</t>
-  </si>
-  <si>
     <t xml:space="preserve">COP mailout </t>
   </si>
   <si>
@@ -222,12 +219,6 @@
     <t>COP 2026</t>
   </si>
   <si>
-    <t>COP 2027</t>
-  </si>
-  <si>
-    <t>COP 2028</t>
-  </si>
-  <si>
     <t>t-shirt size</t>
   </si>
   <si>
@@ -240,7 +231,7 @@
     <t>L</t>
   </si>
   <si>
-    <t>50% approved, 50% in review, working on Phase 2, this is also test how much the text is flowing</t>
+    <t>50% approved, 50% in review, working on Phase 2, this is also test how much the text is flowing. Normally this wouldn't be this long</t>
   </si>
 </sst>
 </file>
@@ -677,7 +668,7 @@
   <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="A3" sqref="A3:A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
@@ -719,27 +710,27 @@
         <v>7</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:9" s="3" customFormat="1" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="F3" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
@@ -747,362 +738,362 @@
     </row>
     <row r="4" spans="1:9" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="F4" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>15</v>
-      </c>
       <c r="E5" s="1" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D6" s="1" t="s">
+      <c r="E6" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E6" s="1" t="s">
-        <v>20</v>
-      </c>
       <c r="F6" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="F7" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D8" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E8" s="1" t="s">
-        <v>20</v>
-      </c>
       <c r="F8" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>8</v>
+        <v>60</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="D9" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E9" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D9" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="F9" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>8</v>
+        <v>60</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="D10" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E10" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D10" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>29</v>
-      </c>
       <c r="F10" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>8</v>
+        <v>60</v>
       </c>
       <c r="B11" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E11" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C11" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>31</v>
-      </c>
       <c r="F11" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B12" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="D12" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E12" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D12" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>34</v>
-      </c>
       <c r="F12" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="C13" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D13" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C13" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D13" s="1" t="s">
+      <c r="E13" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="E13" s="1" t="s">
-        <v>38</v>
-      </c>
       <c r="F13" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="C14" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E14" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C14" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>41</v>
-      </c>
       <c r="F14" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B15" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E15" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C15" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>43</v>
-      </c>
       <c r="F15" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="C16" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E16" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C16" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>46</v>
-      </c>
       <c r="F16" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B17" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E17" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C17" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>48</v>
-      </c>
       <c r="F17" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="C18" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E18" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C18" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>51</v>
-      </c>
       <c r="F18" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="C19" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D19" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="C19" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D19" s="1" t="s">
+      <c r="E19" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="E19" s="1" t="s">
-        <v>55</v>
-      </c>
       <c r="F19" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B20" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E20" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C20" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>57</v>
-      </c>
       <c r="F20" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B21" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="C21" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E21" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="C21" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>60</v>
-      </c>
       <c r="F21" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Filter tasks and switch to individual card view (#3)
* Feat: Add filtering and individual task view

Co-authored-by: nguyentuandanh.7 <nguyentuandanh.7@gmail.com>

* Refactor: Improve layout and card styling in individual mode

Co-authored-by: nguyentuandanh.7 <nguyentuandanh.7@gmail.com>

* Refactor: Adjust styles and add no results message

Co-authored-by: nguyentuandanh.7 <nguyentuandanh.7@gmail.com>

* Add files via upload

* Add dashboard UI and data population logic

Co-authored-by: nguyentuandanh.7 <nguyentuandanh.7@gmail.com>

* Add files via upload

* Refactor: Move filters into content-wrapper and adjust styles

Co-authored-by: nguyentuandanh.7 <nguyentuandanh.7@gmail.com>

* Refactor layout and styling for sidebar and dashboard components

Co-authored-by: nguyentuandanh.7 <nguyentuandanh.7@gmail.com>

---------

Co-authored-by: Cursor Agent <cursoragent@cursor.com>
</commit_message>
<xml_diff>
--- a/data/wip.xlsx
+++ b/data/wip.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\RMIT_WORKS\TEAM\WIP\HTML email\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA2EA3D9-1FCE-4E93-A459-3DE6185C6A79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{101074C1-512C-478B-B4E0-8E6E5C54D1FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="733" yWindow="-118" windowWidth="32898" windowHeight="21181" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="70">
   <si>
     <t>Week 45 (4-11 Nov 2025)</t>
   </si>
@@ -232,6 +232,18 @@
   </si>
   <si>
     <t>50% approved, 50% in review, working on Phase 2, this is also test how much the text is flowing. Normally this wouldn't be this long</t>
+  </si>
+  <si>
+    <t>MED-HIGH</t>
+  </si>
+  <si>
+    <t>Danh project</t>
+  </si>
+  <si>
+    <t>Make this damn thing</t>
+  </si>
+  <si>
+    <t>Hung</t>
   </si>
 </sst>
 </file>
@@ -310,7 +322,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -324,6 +336,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -665,10 +680,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I21"/>
+  <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:A12"/>
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
@@ -692,6 +707,9 @@
       <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="6" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="2" spans="1:9" ht="43.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
@@ -1093,6 +1111,26 @@
         <v>59</v>
       </c>
       <c r="F21" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F22" s="1" t="s">
         <v>62</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Move logo to the right on mobile view (#5)
* Refactor header styles for better responsiveness

Co-authored-by: nguyentuandanh.7 <nguyentuandanh.7@gmail.com>

* Update wip.xlsx

* Update wip.xlsx

---------

Co-authored-by: Cursor Agent <cursoragent@cursor.com>
</commit_message>
<xml_diff>
--- a/data/wip.xlsx
+++ b/data/wip.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\RMIT_WORKS\TEAM\WIP\GIT\RMIT_WIP\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACFBB88D-9CB8-4D40-BDA0-45CA92DAC2C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E1A249E-CDCE-4D38-8149-7DE2E1BA6822}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="733" yWindow="-118" windowWidth="32898" windowHeight="21181" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="65">
   <si>
     <t>Week 45 (4-11 Nov 2025)</t>
   </si>
@@ -219,13 +219,16 @@
     <t>50% approved, 50% in review, working on Phase 2, this is also test how much the text is flowing. Normally this wouldn't be this long</t>
   </si>
   <si>
-    <t>COP 2025</t>
-  </si>
-  <si>
     <t>Med-high</t>
   </si>
   <si>
     <t>Last updated 1 Nov, 15:00</t>
+  </si>
+  <si>
+    <t>Publications 2028</t>
+  </si>
+  <si>
+    <t>Duc</t>
   </si>
 </sst>
 </file>
@@ -272,7 +275,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -291,6 +294,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -304,7 +313,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -319,7 +328,10 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -665,7 +677,7 @@
   <dimension ref="A1:H23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="A3" sqref="A3:A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
@@ -685,11 +697,11 @@
       <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="D1" s="6" t="s">
+      <c r="C1" s="6" t="s">
         <v>62</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="43.55" customHeight="1" x14ac:dyDescent="0.3">
@@ -799,7 +811,7 @@
     </row>
     <row r="8" spans="1:8" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>21</v>
@@ -816,7 +828,7 @@
     </row>
     <row r="9" spans="1:8" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>22</v>
@@ -833,7 +845,7 @@
     </row>
     <row r="10" spans="1:8" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>25</v>
@@ -850,7 +862,7 @@
     </row>
     <row r="11" spans="1:8" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>28</v>
@@ -867,7 +879,7 @@
     </row>
     <row r="12" spans="1:8" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>30</v>
@@ -1036,7 +1048,21 @@
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A22" s="2"/>
+      <c r="A22" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="2"/>

</xml_diff>